<commit_message>
Analisis 5, 6, 7 y 8 hechos.
</commit_message>
<xml_diff>
--- a/data/plantilla.xlsx
+++ b/data/plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josemaria.flores\Documents\CEDIS\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2042969F-4F91-4EA4-A46D-357A0131BC4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89BD666-CEF5-4444-9841-4635F9C1A44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6A017247-C418-4239-B6E8-A667328D32B4}"/>
+    <workbookView xWindow="3630" yWindow="5040" windowWidth="12600" windowHeight="8580" firstSheet="3" activeTab="4" xr2:uid="{6A017247-C418-4239-B6E8-A667328D32B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Información SKU" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
-  <si>
-    <t>Clave</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Nombre SKU</t>
   </si>
@@ -55,15 +52,6 @@
     <t>Política de Inventario</t>
   </si>
   <si>
-    <t>Volumen x Pieza</t>
-  </si>
-  <si>
-    <t>Peso x Pieza</t>
-  </si>
-  <si>
-    <t>Piezas x Caja</t>
-  </si>
-  <si>
     <t>Peso x Caja</t>
   </si>
   <si>
@@ -206,6 +194,15 @@
   </si>
   <si>
     <t>Turno Devolución</t>
+  </si>
+  <si>
+    <t>Volumen x Unidad</t>
+  </si>
+  <si>
+    <t>Peso x Unidad</t>
+  </si>
+  <si>
+    <t>Unidades x Caja</t>
   </si>
 </sst>
 </file>
@@ -289,10 +286,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,22 +590,22 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -628,67 +621,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -720,25 +713,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -753,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,40 +768,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +816,7 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -849,52 +842,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -909,8 +902,8 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,52 +928,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcionalidad agregada a analisis de 0 al 4
</commit_message>
<xml_diff>
--- a/data/plantilla.xlsx
+++ b/data/plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josemaria.flores\Documents\CEDIS\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89BD666-CEF5-4444-9841-4635F9C1A44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA407D2-2438-4BE6-80FC-0AEE31121283}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="5040" windowWidth="12600" windowHeight="8580" firstSheet="3" activeTab="4" xr2:uid="{6A017247-C418-4239-B6E8-A667328D32B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6A017247-C418-4239-B6E8-A667328D32B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Información SKU" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Base de Embarque" sheetId="4" r:id="rId4"/>
     <sheet name="Base de Devoluciones" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterateCount="1" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,16 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
-  <si>
-    <t>Nombre SKU</t>
-  </si>
-  <si>
-    <t>Clasificación ABC Cliente</t>
-  </si>
-  <si>
-    <t>Clasificación ABC Sintec</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Política de Inventario</t>
   </si>
@@ -61,27 +52,12 @@
     <t>Cajas x Tarima</t>
   </si>
   <si>
-    <t>ID Categoría</t>
-  </si>
-  <si>
     <t>Categoría</t>
   </si>
   <si>
-    <t>ID Subcategoría</t>
-  </si>
-  <si>
     <t>Sub-Categoría</t>
   </si>
   <si>
-    <t>Familia Almacén I</t>
-  </si>
-  <si>
-    <t>Familia Almacén II</t>
-  </si>
-  <si>
-    <t>Familia Almacén III</t>
-  </si>
-  <si>
     <t>Zona de Completitud</t>
   </si>
   <si>
@@ -91,12 +67,6 @@
     <t>Densidad de Pickeo</t>
   </si>
   <si>
-    <t>ID Producto</t>
-  </si>
-  <si>
-    <t>Descripción Producto</t>
-  </si>
-  <si>
     <t>Unidades de Inventario</t>
   </si>
   <si>
@@ -106,18 +76,6 @@
     <t>Tarimas de Inventario</t>
   </si>
   <si>
-    <t>Semana</t>
-  </si>
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>ID Proveedor</t>
-  </si>
-  <si>
-    <t>Nombre Proveedor</t>
-  </si>
-  <si>
     <t>Pedido</t>
   </si>
   <si>
@@ -133,33 +91,6 @@
     <t>Tarimas Recibidas</t>
   </si>
   <si>
-    <t>Fecha Recibo</t>
-  </si>
-  <si>
-    <t>Horario Recibo</t>
-  </si>
-  <si>
-    <t>Turno Recibo</t>
-  </si>
-  <si>
-    <t>ID Canal</t>
-  </si>
-  <si>
-    <t>Canal</t>
-  </si>
-  <si>
-    <t>ID Cliente</t>
-  </si>
-  <si>
-    <t>Nombre Cliente</t>
-  </si>
-  <si>
-    <t>ID Destino</t>
-  </si>
-  <si>
-    <t>Nombre Destino</t>
-  </si>
-  <si>
     <t>Unidades Embarcadas</t>
   </si>
   <si>
@@ -169,15 +100,6 @@
     <t>Tarimas Embarcadas</t>
   </si>
   <si>
-    <t>Fecha Embarque</t>
-  </si>
-  <si>
-    <t>Horario Embarque</t>
-  </si>
-  <si>
-    <t>Turno Embarque</t>
-  </si>
-  <si>
     <t>Unidades Devueltas</t>
   </si>
   <si>
@@ -187,15 +109,6 @@
     <t>Tarimas Devueltas</t>
   </si>
   <si>
-    <t>Fecha Devolución</t>
-  </si>
-  <si>
-    <t>Horario Devolución</t>
-  </si>
-  <si>
-    <t>Turno Devolución</t>
-  </si>
-  <si>
     <t>Volumen x Unidad</t>
   </si>
   <si>
@@ -203,6 +116,90 @@
   </si>
   <si>
     <t>Unidades x Caja</t>
+  </si>
+  <si>
+    <t>ID del Producto</t>
+  </si>
+  <si>
+    <t>Descripción del Producto</t>
+  </si>
+  <si>
+    <t>Clasificación ABC del Cliente</t>
+  </si>
+  <si>
+    <t>Clasificación ABC de Sintec</t>
+  </si>
+  <si>
+    <t>ID de la Categoría</t>
+  </si>
+  <si>
+    <t>ID de la Sub-Categoría</t>
+  </si>
+  <si>
+    <t>Familia de Almacén I</t>
+  </si>
+  <si>
+    <t>Familia de Almacén II</t>
+  </si>
+  <si>
+    <t>Familia de Almacén III</t>
+  </si>
+  <si>
+    <t>Fecha de Inventario</t>
+  </si>
+  <si>
+    <t>Hora de Inventario</t>
+  </si>
+  <si>
+    <t>ID del Proveedor</t>
+  </si>
+  <si>
+    <t>Nombre del Proveedor</t>
+  </si>
+  <si>
+    <t>Fecha de Recibo</t>
+  </si>
+  <si>
+    <t>Hora de Recibo</t>
+  </si>
+  <si>
+    <t>Turno de Recibo</t>
+  </si>
+  <si>
+    <t>ID del Canal</t>
+  </si>
+  <si>
+    <t>Nombre del Canal</t>
+  </si>
+  <si>
+    <t>ID del Cliente</t>
+  </si>
+  <si>
+    <t>Nombre del Cliente</t>
+  </si>
+  <si>
+    <t>ID del Destino</t>
+  </si>
+  <si>
+    <t>Nombre del Destino</t>
+  </si>
+  <si>
+    <t>Fecha de Embarque</t>
+  </si>
+  <si>
+    <t>Hora de Embarque</t>
+  </si>
+  <si>
+    <t>Turno de Embarque</t>
+  </si>
+  <si>
+    <t>Fecha de Devolución</t>
+  </si>
+  <si>
+    <t>Hora de Devolución</t>
+  </si>
+  <si>
+    <t>Turno de Devolución</t>
   </si>
 </sst>
 </file>
@@ -220,23 +217,18 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -249,31 +241,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -591,15 +586,15 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -607,13 +602,13 @@
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -621,67 +616,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -697,41 +692,41 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -746,62 +741,62 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -816,78 +811,78 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -902,78 +897,78 @@
   </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
+      <c r="A1" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>